<commit_message>
Updating file paths to be relative and one change in a variable type in main HHData, affecting data dictionary and main.RData
</commit_message>
<xml_diff>
--- a/Data Dictionary/HH_DataDictionary.xlsx
+++ b/Data Dictionary/HH_DataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmcr\Documents\ARMS_Golden\HHData\Raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmcr\Documents\ARMS_Golden_Git\SW-Madagascar\Data Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5C9EE8-478D-4220-B6FB-0DED6A36E629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8730A7-13B2-4E7C-84E5-6419A29CE234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1833" yWindow="1833" windowWidth="19200" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2540" yWindow="2540" windowWidth="19200" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -2272,8 +2272,8 @@
   </sheetPr>
   <dimension ref="A1:G887"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3375,7 +3375,7 @@
         <v>142</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>28</v>
@@ -11033,7 +11033,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>489</v>
       </c>
@@ -11047,7 +11047,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>489</v>
       </c>
@@ -11061,7 +11061,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>489</v>
       </c>
@@ -11075,7 +11075,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>489</v>
       </c>
@@ -11089,7 +11089,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>489</v>
       </c>
@@ -11103,7 +11103,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>489</v>
       </c>
@@ -11117,7 +11117,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>489</v>
       </c>
@@ -11131,7 +11131,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>489</v>
       </c>
@@ -11145,7 +11145,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>489</v>
       </c>
@@ -11159,7 +11159,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>489</v>
       </c>
@@ -11276,7 +11276,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>514</v>
       </c>
@@ -11290,7 +11290,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>514</v>
       </c>
@@ -11304,7 +11304,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>514</v>
       </c>
@@ -11318,7 +11318,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>514</v>
       </c>
@@ -11332,7 +11332,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>514</v>
       </c>
@@ -11346,7 +11346,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>514</v>
       </c>
@@ -11360,7 +11360,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>514</v>
       </c>
@@ -11374,7 +11374,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>514</v>
       </c>
@@ -11388,7 +11388,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>514</v>
       </c>
@@ -11402,7 +11402,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>514</v>
       </c>
@@ -11416,7 +11416,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>514</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>514</v>
       </c>
@@ -12213,7 +12213,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>556</v>
       </c>
@@ -12227,7 +12227,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>556</v>
       </c>
@@ -12241,7 +12241,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>556</v>
       </c>
@@ -12255,7 +12255,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>556</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>556</v>
       </c>
@@ -12283,7 +12283,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>556</v>
       </c>
@@ -12297,7 +12297,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>556</v>
       </c>
@@ -12311,7 +12311,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>556</v>
       </c>
@@ -12325,7 +12325,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>556</v>
       </c>
@@ -12339,7 +12339,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>556</v>
       </c>
@@ -12353,7 +12353,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>556</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>556</v>
       </c>
@@ -12530,7 +12530,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>561</v>
       </c>
@@ -12544,7 +12544,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>561</v>
       </c>
@@ -12558,7 +12558,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>561</v>
       </c>
@@ -12572,7 +12572,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>561</v>
       </c>
@@ -12586,7 +12586,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>561</v>
       </c>
@@ -12600,7 +12600,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>561</v>
       </c>
@@ -12614,7 +12614,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>561</v>
       </c>
@@ -12628,7 +12628,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>561</v>
       </c>
@@ -12642,7 +12642,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>561</v>
       </c>
@@ -12656,7 +12656,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>561</v>
       </c>
@@ -12793,7 +12793,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>575</v>
       </c>
@@ -12807,7 +12807,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>575</v>
       </c>
@@ -12821,7 +12821,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>575</v>
       </c>
@@ -12835,7 +12835,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>575</v>
       </c>
@@ -12849,7 +12849,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>575</v>
       </c>
@@ -12863,7 +12863,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>575</v>
       </c>
@@ -12877,7 +12877,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>575</v>
       </c>
@@ -12891,7 +12891,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>575</v>
       </c>
@@ -12905,7 +12905,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>575</v>
       </c>
@@ -12919,7 +12919,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>575</v>
       </c>
@@ -12933,7 +12933,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>575</v>
       </c>
@@ -12947,7 +12947,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>575</v>
       </c>

</xml_diff>

<commit_message>
Adding data collection wave variable
</commit_message>
<xml_diff>
--- a/Data Dictionary/HH_DataDictionary.xlsx
+++ b/Data Dictionary/HH_DataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmcr\Documents\ARMS_Golden_Git\SW-Madagascar\Data Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8730A7-13B2-4E7C-84E5-6419A29CE234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BC6D77-1005-464F-AF9E-EA0A9110DAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="2540" windowWidth="19200" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="661">
   <si>
     <t>dataset</t>
   </si>
@@ -2003,6 +2003,18 @@
   </si>
   <si>
     <t>_III_Questions_about_domestic_animals</t>
+  </si>
+  <si>
+    <t>collection_wave</t>
+  </si>
+  <si>
+    <t>Data collection wave</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>Derived variable. 99 indicates the date is outside indicated collection times</t>
   </si>
 </sst>
 </file>
@@ -2270,10 +2282,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G887"/>
+  <dimension ref="A1:G888"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2341,29 +2353,32 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>657</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>658</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>659</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2373,13 +2388,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2389,10 +2404,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>17</v>
@@ -2405,10 +2420,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>17</v>
@@ -2421,10 +2436,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
@@ -2437,17 +2452,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -2455,13 +2468,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -2473,10 +2486,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>31</v>
@@ -2491,10 +2504,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>31</v>
@@ -2509,15 +2522,17 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -2525,17 +2540,15 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -2543,10 +2556,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>31</v>
@@ -2561,40 +2574,37 @@
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="D18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
-      <c r="A18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -2602,111 +2612,116 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F19" s="1"/>
+      <c r="G19" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="2" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="21" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="1"/>
+      <c r="G21" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="23" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F23" s="1"/>
+      <c r="G23" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -2714,17 +2729,15 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -2732,10 +2745,10 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>31</v>
@@ -2750,10 +2763,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>31</v>
@@ -2761,40 +2774,40 @@
       <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>28</v>
@@ -2806,15 +2819,17 @@
         <v>7</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -2822,17 +2837,15 @@
         <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -2840,10 +2853,10 @@
         <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>31</v>
@@ -2858,10 +2871,10 @@
         <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>31</v>
@@ -2869,19 +2882,17 @@
       <c r="E33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>31</v>
@@ -2889,17 +2900,19 @@
       <c r="E34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>31</v>
@@ -2907,37 +2920,37 @@
       <c r="E35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>17</v>
@@ -2945,78 +2958,78 @@
       <c r="E37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>656</v>
+        <v>93</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>97</v>
+        <v>656</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -3024,10 +3037,10 @@
         <v>7</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>17</v>
@@ -3042,10 +3055,10 @@
         <v>7</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>17</v>
@@ -3060,10 +3073,10 @@
         <v>7</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>17</v>
@@ -3078,10 +3091,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>17</v>
@@ -3096,10 +3109,10 @@
         <v>7</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>17</v>
@@ -3114,10 +3127,10 @@
         <v>7</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>17</v>
@@ -3132,10 +3145,10 @@
         <v>7</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>17</v>
@@ -3150,10 +3163,10 @@
         <v>7</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>17</v>
@@ -3168,10 +3181,10 @@
         <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>17</v>
@@ -3186,10 +3199,10 @@
         <v>7</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>17</v>
@@ -3204,10 +3217,10 @@
         <v>7</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>17</v>
@@ -3222,10 +3235,10 @@
         <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>17</v>
@@ -3240,10 +3253,10 @@
         <v>7</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>17</v>
@@ -3258,10 +3271,10 @@
         <v>7</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>17</v>
@@ -3270,42 +3283,42 @@
         <v>28</v>
       </c>
       <c r="F55" s="1"/>
-      <c r="G55" s="2" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="56" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E56" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F56" s="1"/>
+      <c r="G56" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -3313,10 +3326,10 @@
         <v>7</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>31</v>
@@ -3331,10 +3344,10 @@
         <v>7</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>31</v>
@@ -3342,19 +3355,17 @@
       <c r="E59" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>31</v>
@@ -3362,17 +3373,19 @@
       <c r="E60" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F60" s="1"/>
+      <c r="F60" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="61" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>31</v>
@@ -3380,28 +3393,26 @@
       <c r="E61" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>143</v>
-      </c>
+      <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -3409,10 +3420,10 @@
         <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>17</v>
@@ -3421,7 +3432,7 @@
         <v>28</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -3429,33 +3440,37 @@
         <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F64" s="1"/>
+      <c r="F64" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="65" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E65" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -3463,17 +3478,15 @@
         <v>7</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -3481,10 +3494,10 @@
         <v>7</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>31</v>
@@ -3499,10 +3512,10 @@
         <v>7</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>31</v>
@@ -3511,19 +3524,16 @@
         <v>28</v>
       </c>
       <c r="F68" s="1"/>
-      <c r="G68" s="2" t="s">
-        <v>160</v>
-      </c>
     </row>
     <row r="69" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>31</v>
@@ -3531,8 +3541,9 @@
       <c r="E69" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>163</v>
+      <c r="F69" s="1"/>
+      <c r="G69" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -3540,27 +3551,31 @@
         <v>7</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C70" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="D70" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="71" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>166</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="C71" s="1"/>
       <c r="D71" s="2" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -3570,31 +3585,26 @@
         <v>7</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-      <c r="G72" s="2" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="73" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A73" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>31</v>
@@ -3602,8 +3612,9 @@
       <c r="E73" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>172</v>
+      <c r="F73" s="1"/>
+      <c r="G73" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -3611,27 +3622,31 @@
         <v>7</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C74" s="1"/>
+        <v>170</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="D74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="75" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>175</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C75" s="1"/>
       <c r="D75" s="2" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -3641,10 +3656,10 @@
         <v>7</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>62</v>
@@ -3657,17 +3672,15 @@
         <v>7</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
@@ -3675,33 +3688,31 @@
         <v>7</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>182</v>
-      </c>
+      <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>28</v>
@@ -3715,10 +3726,10 @@
         <v>7</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>31</v>
@@ -3735,31 +3746,33 @@
         <v>7</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F81" s="1"/>
+      <c r="F81" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="82" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A82" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>28</v>
@@ -3771,647 +3784,645 @@
         <v>7</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>193</v>
-      </c>
+      <c r="F83" s="1"/>
     </row>
     <row r="84" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A84" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F84" s="1"/>
+      <c r="F84" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="85" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>198</v>
-      </c>
+      <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A86" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F86" s="1"/>
+      <c r="F86" s="1" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="87" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A87" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>203</v>
-      </c>
+      <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A88" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F88" s="1"/>
+      <c r="F88" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="89" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A89" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>208</v>
-      </c>
+      <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A90" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F90" s="1"/>
+      <c r="F90" s="1" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="91" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A91" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>213</v>
-      </c>
+      <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A92" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F92" s="1"/>
+      <c r="F92" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="93" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A93" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>218</v>
-      </c>
+      <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A94" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F94" s="1"/>
+      <c r="F94" s="1" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="95" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A95" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A96" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F96" s="1"/>
+      <c r="F96" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="97" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A97" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>228</v>
-      </c>
+      <c r="F97" s="1"/>
     </row>
     <row r="98" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A98" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F98" s="1"/>
+      <c r="F98" s="1" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="99" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A99" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F99" s="1"/>
     </row>
     <row r="100" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A100" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F100" s="1"/>
+      <c r="F100" s="1" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="101" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A101" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F101" s="1" t="s">
-        <v>238</v>
-      </c>
+      <c r="F101" s="1"/>
     </row>
     <row r="102" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A102" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F102" s="1"/>
+      <c r="F102" s="1" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="103" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A103" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F103" s="1" t="s">
-        <v>243</v>
-      </c>
+      <c r="F103" s="1"/>
     </row>
     <row r="104" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A104" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F104" s="1"/>
+      <c r="F104" s="1" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="105" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A105" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F105" s="1" t="s">
-        <v>248</v>
-      </c>
+      <c r="F105" s="1"/>
     </row>
     <row r="106" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A106" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F106" s="1"/>
+      <c r="F106" s="1" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="107" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F107" s="1" t="s">
-        <v>253</v>
-      </c>
+      <c r="F107" s="1"/>
     </row>
     <row r="108" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A108" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F108" s="1"/>
+      <c r="F108" s="1" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="109" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A109" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F109" s="1" t="s">
-        <v>258</v>
-      </c>
+      <c r="F109" s="1"/>
     </row>
     <row r="110" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A110" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F110" s="1"/>
+      <c r="F110" s="1" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="111" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A111" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F111" s="1" t="s">
-        <v>263</v>
-      </c>
+      <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A112" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F112" s="1"/>
+      <c r="F112" s="1" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="113" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A113" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F113" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="F113" s="1"/>
     </row>
     <row r="114" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A114" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F114" s="1"/>
+      <c r="F114" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="115" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A115" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>273</v>
-      </c>
+      <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A116" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -4419,19 +4430,19 @@
         <v>7</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -4439,19 +4450,19 @@
         <v>7</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -4459,19 +4470,19 @@
         <v>7</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -4479,19 +4490,19 @@
         <v>7</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -4499,19 +4510,19 @@
         <v>7</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -4519,132 +4530,136 @@
         <v>7</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F122" s="1"/>
+      <c r="F122" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="123" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A123" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F123" s="1" t="s">
-        <v>296</v>
-      </c>
+      <c r="F123" s="1"/>
     </row>
     <row r="124" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A124" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E124" s="1"/>
-      <c r="F124" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="125" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A125" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E125" s="1"/>
-      <c r="F125" s="1" t="s">
-        <v>301</v>
-      </c>
+      <c r="F125" s="1"/>
     </row>
     <row r="126" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A126" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E126" s="1"/>
-      <c r="F126" s="1"/>
+      <c r="F126" s="1" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="127" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A127" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E127" s="1"/>
-      <c r="F127" s="1" t="s">
-        <v>306</v>
-      </c>
+      <c r="F127" s="1"/>
     </row>
     <row r="128" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A128" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="E128" s="1"/>
-      <c r="F128" s="1"/>
+      <c r="F128" s="1" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="129" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A129" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>62</v>
@@ -4657,17 +4672,15 @@
         <v>7</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E130" s="1"/>
       <c r="F130" s="1"/>
     </row>
     <row r="131" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -4675,10 +4688,10 @@
         <v>7</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>31</v>
@@ -4693,10 +4706,10 @@
         <v>7</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>31</v>
@@ -4711,10 +4724,10 @@
         <v>7</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>31</v>
@@ -4729,10 +4742,10 @@
         <v>7</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>31</v>
@@ -4747,10 +4760,10 @@
         <v>7</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>31</v>
@@ -4765,10 +4778,10 @@
         <v>7</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>31</v>
@@ -4783,10 +4796,10 @@
         <v>7</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>31</v>
@@ -4801,15 +4814,17 @@
         <v>7</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E138" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F138" s="1"/>
     </row>
     <row r="139" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -4817,17 +4832,15 @@
         <v>7</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E139" s="1"/>
       <c r="F139" s="1"/>
     </row>
     <row r="140" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -4835,10 +4848,10 @@
         <v>7</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>31</v>
@@ -4853,10 +4866,10 @@
         <v>7</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>31</v>
@@ -4871,10 +4884,10 @@
         <v>7</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>31</v>
@@ -4889,10 +4902,10 @@
         <v>7</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>31</v>
@@ -4907,10 +4920,10 @@
         <v>7</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>31</v>
@@ -4925,10 +4938,10 @@
         <v>7</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>31</v>
@@ -4943,10 +4956,10 @@
         <v>7</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>31</v>
@@ -4961,10 +4974,10 @@
         <v>7</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>31</v>
@@ -4979,10 +4992,10 @@
         <v>7</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>31</v>
@@ -4997,10 +5010,10 @@
         <v>7</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>31</v>
@@ -5015,10 +5028,10 @@
         <v>7</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>31</v>
@@ -5033,10 +5046,10 @@
         <v>7</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>31</v>
@@ -5051,10 +5064,10 @@
         <v>7</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>31</v>
@@ -5069,15 +5082,17 @@
         <v>7</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E153" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F153" s="1"/>
     </row>
     <row r="154" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -5085,10 +5100,10 @@
         <v>7</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>62</v>
@@ -5101,17 +5116,15 @@
         <v>7</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E155" s="1"/>
       <c r="F155" s="1"/>
     </row>
     <row r="156" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -5119,10 +5132,10 @@
         <v>7</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>31</v>
@@ -5137,10 +5150,10 @@
         <v>7</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>31</v>
@@ -5155,15 +5168,17 @@
         <v>7</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E158" s="1"/>
+      <c r="E158" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F158" s="1"/>
     </row>
     <row r="159" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -5171,13 +5186,13 @@
         <v>7</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
@@ -5187,17 +5202,15 @@
         <v>7</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E160" s="1"/>
       <c r="F160" s="1"/>
     </row>
     <row r="161" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -5205,10 +5218,10 @@
         <v>7</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>31</v>
@@ -5223,10 +5236,10 @@
         <v>7</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>31</v>
@@ -5234,19 +5247,17 @@
       <c r="E162" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F162" s="1" t="s">
-        <v>377</v>
-      </c>
+      <c r="F162" s="1"/>
     </row>
     <row r="163" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A163" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>31</v>
@@ -5254,17 +5265,19 @@
       <c r="E163" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F163" s="1"/>
+      <c r="F163" s="1" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="164" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A164" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>31</v>
@@ -5279,10 +5292,10 @@
         <v>7</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>31</v>
@@ -5297,10 +5310,10 @@
         <v>7</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>31</v>
@@ -5315,10 +5328,10 @@
         <v>7</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>31</v>
@@ -5326,19 +5339,17 @@
       <c r="E167" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F167" s="1" t="s">
-        <v>388</v>
-      </c>
+      <c r="F167" s="1"/>
     </row>
     <row r="168" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A168" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>31</v>
@@ -5355,10 +5366,10 @@
         <v>7</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>31</v>
@@ -5366,17 +5377,19 @@
       <c r="E169" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F169" s="1"/>
+      <c r="F169" s="1" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="170" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A170" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>31</v>
@@ -5391,10 +5404,10 @@
         <v>7</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>31</v>
@@ -5402,28 +5415,26 @@
       <c r="E171" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F171" s="1" t="s">
-        <v>397</v>
-      </c>
+      <c r="F171" s="1"/>
     </row>
     <row r="172" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A172" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -5431,10 +5442,10 @@
         <v>7</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>17</v>
@@ -5442,17 +5453,19 @@
       <c r="E173" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F173" s="1"/>
+      <c r="F173" s="1" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="174" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A174" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>17</v>
@@ -5467,15 +5480,17 @@
         <v>7</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E175" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F175" s="1"/>
     </row>
     <row r="176" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -5483,17 +5498,15 @@
         <v>7</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E176" s="1"/>
       <c r="F176" s="1"/>
     </row>
     <row r="177" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -5501,10 +5514,10 @@
         <v>7</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>31</v>
@@ -5519,10 +5532,10 @@
         <v>7</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>31</v>
@@ -5537,10 +5550,10 @@
         <v>7</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>31</v>
@@ -5555,10 +5568,10 @@
         <v>7</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>31</v>
@@ -5573,10 +5586,10 @@
         <v>7</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>31</v>
@@ -5591,10 +5604,10 @@
         <v>7</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>31</v>
@@ -5609,10 +5622,10 @@
         <v>7</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>31</v>
@@ -5627,10 +5640,10 @@
         <v>7</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>31</v>
@@ -5645,10 +5658,10 @@
         <v>7</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>31</v>
@@ -5663,10 +5676,10 @@
         <v>7</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>31</v>
@@ -5681,10 +5694,10 @@
         <v>7</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>31</v>
@@ -5699,15 +5712,17 @@
         <v>7</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E188" s="1"/>
+      <c r="E188" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F188" s="1"/>
     </row>
     <row r="189" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -5715,318 +5730,316 @@
         <v>7</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E189" s="1"/>
-      <c r="F189" s="1" t="s">
-        <v>435</v>
-      </c>
+      <c r="F189" s="1"/>
     </row>
     <row r="190" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A190" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E190" s="1"/>
-      <c r="F190" s="1"/>
+      <c r="F190" s="1" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="191" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A191" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E191" s="1"/>
-      <c r="F191" s="1" t="s">
-        <v>440</v>
-      </c>
+      <c r="F191" s="1"/>
     </row>
     <row r="192" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A192" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E192" s="1"/>
-      <c r="F192" s="1"/>
+      <c r="F192" s="1" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="193" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A193" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E193" s="1"/>
-      <c r="F193" s="1" t="s">
-        <v>445</v>
-      </c>
+      <c r="F193" s="1"/>
     </row>
     <row r="194" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A194" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E194" s="1"/>
-      <c r="F194" s="1"/>
+      <c r="F194" s="1" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="195" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A195" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E195" s="1"/>
-      <c r="F195" s="1" t="s">
-        <v>449</v>
-      </c>
+      <c r="F195" s="1"/>
     </row>
     <row r="196" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A196" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E196" s="1"/>
-      <c r="F196" s="1"/>
+      <c r="F196" s="1" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="197" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A197" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E197" s="1"/>
-      <c r="F197" s="1" t="s">
-        <v>453</v>
-      </c>
+      <c r="F197" s="1"/>
     </row>
     <row r="198" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A198" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E198" s="1"/>
-      <c r="F198" s="1"/>
+      <c r="F198" s="1" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="199" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A199" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>444</v>
+        <v>455</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E199" s="1"/>
-      <c r="F199" s="1" t="s">
-        <v>457</v>
-      </c>
+      <c r="F199" s="1"/>
     </row>
     <row r="200" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A200" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E200" s="1"/>
-      <c r="F200" s="1"/>
+      <c r="F200" s="1" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="201" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A201" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>444</v>
+        <v>459</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E201" s="1"/>
-      <c r="F201" s="1" t="s">
-        <v>461</v>
-      </c>
+      <c r="F201" s="1"/>
     </row>
     <row r="202" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A202" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E202" s="1"/>
-      <c r="F202" s="1"/>
+      <c r="F202" s="1" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="203" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A203" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>444</v>
+        <v>463</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E203" s="1"/>
-      <c r="F203" s="1" t="s">
-        <v>465</v>
-      </c>
+      <c r="F203" s="1"/>
     </row>
     <row r="204" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A204" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E204" s="1"/>
-      <c r="F204" s="1"/>
+      <c r="F204" s="1" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="205" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A205" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>444</v>
+        <v>467</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E205" s="1"/>
-      <c r="F205" s="1" t="s">
-        <v>469</v>
-      </c>
+      <c r="F205" s="1"/>
     </row>
     <row r="206" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A206" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>471</v>
+        <v>444</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E206" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F206" s="1"/>
+      <c r="E206" s="1"/>
+      <c r="F206" s="1" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="207" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A207" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>31</v>
@@ -6034,19 +6047,17 @@
       <c r="E207" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F207" s="1" t="s">
-        <v>474</v>
-      </c>
+      <c r="F207" s="1"/>
     </row>
     <row r="208" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A208" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>31</v>
@@ -6054,22 +6065,26 @@
       <c r="E208" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F208" s="1"/>
+      <c r="F208" s="1" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="209" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A209" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E209" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F209" s="1"/>
     </row>
     <row r="210" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -6077,11 +6092,13 @@
         <v>7</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="C210" s="1"/>
+        <v>477</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>478</v>
+      </c>
       <c r="D210" s="2" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="E210" s="1"/>
       <c r="F210" s="1"/>
@@ -6091,11 +6108,11 @@
         <v>7</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C211" s="1"/>
       <c r="D211" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E211" s="1"/>
       <c r="F211" s="1"/>
@@ -6105,11 +6122,11 @@
         <v>7</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C212" s="1"/>
       <c r="D212" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E212" s="1"/>
       <c r="F212" s="1"/>
@@ -6119,11 +6136,11 @@
         <v>7</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C213" s="1"/>
       <c r="D213" s="2" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="E213" s="1"/>
       <c r="F213" s="1"/>
@@ -6133,7 +6150,7 @@
         <v>7</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C214" s="1"/>
       <c r="D214" s="2" t="s">
@@ -6147,11 +6164,11 @@
         <v>7</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C215" s="1"/>
       <c r="D215" s="2" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="E215" s="1"/>
       <c r="F215" s="1"/>
@@ -6161,7 +6178,7 @@
         <v>7</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C216" s="1"/>
       <c r="D216" s="2" t="s">
@@ -6175,7 +6192,7 @@
         <v>7</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C217" s="1"/>
       <c r="D217" s="2" t="s">
@@ -6189,11 +6206,11 @@
         <v>7</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C218" s="1"/>
       <c r="D218" s="2" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="E218" s="1"/>
       <c r="F218" s="1"/>
@@ -6203,19 +6220,26 @@
         <v>7</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C219" s="1"/>
       <c r="D219" s="2" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="E219" s="1"/>
       <c r="F219" s="1"/>
     </row>
     <row r="220" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
-      <c r="A220" s="1"/>
-      <c r="B220" s="1"/>
+      <c r="A220" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="C220" s="1"/>
+      <c r="D220" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E220" s="1"/>
       <c r="F220" s="1"/>
     </row>
@@ -10887,6 +10911,13 @@
       <c r="C887" s="1"/>
       <c r="E887" s="1"/>
       <c r="F887" s="1"/>
+    </row>
+    <row r="888" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A888" s="1"/>
+      <c r="B888" s="1"/>
+      <c r="C888" s="1"/>
+      <c r="E888" s="1"/>
+      <c r="F888" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixing some variable translations
</commit_message>
<xml_diff>
--- a/Data Dictionary/HH_DataDictionary.xlsx
+++ b/Data Dictionary/HH_DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmcr\Documents\ARMS_Golden_Git\SW-Madagascar\Data Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BC6D77-1005-464F-AF9E-EA0A9110DAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C81FCB-DD4F-497F-8E5D-B145C293E45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="665">
   <si>
     <t>dataset</t>
   </si>
@@ -2015,6 +2015,18 @@
   </si>
   <si>
     <t>Derived variable. 99 indicates the date is outside indicated collection times</t>
+  </si>
+  <si>
+    <t>translation_format</t>
+  </si>
+  <si>
+    <t>mesure</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>wage</t>
   </si>
 </sst>
 </file>
@@ -2282,10 +2294,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G888"/>
+  <dimension ref="A1:H888"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2293,7 +2305,7 @@
     <col min="2" max="2" width="29.64453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2315,8 +2327,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H1" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2332,7 +2347,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2348,7 +2363,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2367,7 +2382,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2383,7 +2398,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2399,7 +2414,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2415,7 +2430,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2431,7 +2446,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2447,7 +2462,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2463,7 +2478,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2481,7 +2496,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -2499,7 +2514,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2517,7 +2532,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -2535,7 +2550,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -2551,7 +2566,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -3455,7 +3470,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -3473,7 +3488,7 @@
       </c>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
@@ -3489,7 +3504,7 @@
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -3507,7 +3522,7 @@
       </c>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A68" s="1" t="s">
         <v>7</v>
       </c>
@@ -3525,7 +3540,7 @@
       </c>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A69" s="1" t="s">
         <v>7</v>
       </c>
@@ -3545,8 +3560,11 @@
       <c r="G69" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="H69" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A70" s="1" t="s">
         <v>7</v>
       </c>
@@ -3566,7 +3584,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
         <v>7</v>
       </c>
@@ -3580,7 +3598,7 @@
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A72" s="1" t="s">
         <v>7</v>
       </c>
@@ -3596,7 +3614,7 @@
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A73" s="1" t="s">
         <v>7</v>
       </c>
@@ -3617,7 +3635,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A74" s="1" t="s">
         <v>7</v>
       </c>
@@ -3637,7 +3655,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A75" s="1" t="s">
         <v>7</v>
       </c>
@@ -3651,7 +3669,7 @@
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
@@ -3667,7 +3685,7 @@
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
@@ -3683,7 +3701,7 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A78" s="1" t="s">
         <v>7</v>
       </c>
@@ -3701,7 +3719,7 @@
       </c>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
         <v>7</v>
       </c>
@@ -3721,7 +3739,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -10929,13 +10947,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10957,8 +10977,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H1" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>489</v>
       </c>
@@ -10975,8 +10998,11 @@
         <v>28</v>
       </c>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H2" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>489</v>
       </c>
@@ -10994,7 +11020,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>489</v>
       </c>
@@ -11012,7 +11038,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>489</v>
       </c>
@@ -11030,7 +11056,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>489</v>
       </c>
@@ -11045,8 +11071,11 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H6" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>489</v>
       </c>
@@ -11064,7 +11093,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>489</v>
       </c>
@@ -11078,7 +11107,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>489</v>
       </c>
@@ -11092,7 +11121,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>489</v>
       </c>
@@ -11106,7 +11135,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>489</v>
       </c>
@@ -11120,7 +11149,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>489</v>
       </c>
@@ -11134,7 +11163,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>489</v>
       </c>
@@ -11148,7 +11177,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>489</v>
       </c>
@@ -11162,7 +11191,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>489</v>
       </c>
@@ -11176,7 +11205,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>489</v>
       </c>
@@ -11242,13 +11271,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11270,8 +11301,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H1" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>514</v>
       </c>
@@ -11289,7 +11323,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>514</v>
       </c>
@@ -11307,7 +11341,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>514</v>
       </c>
@@ -11321,7 +11355,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>514</v>
       </c>
@@ -11335,7 +11369,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>514</v>
       </c>
@@ -11349,7 +11383,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>514</v>
       </c>
@@ -11363,7 +11397,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>514</v>
       </c>
@@ -11377,7 +11411,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>514</v>
       </c>
@@ -11391,7 +11425,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>514</v>
       </c>
@@ -11405,7 +11439,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>514</v>
       </c>
@@ -11419,7 +11453,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>514</v>
       </c>
@@ -11433,7 +11467,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>514</v>
       </c>
@@ -11447,7 +11481,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>514</v>
       </c>
@@ -11461,7 +11495,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>514</v>
       </c>
@@ -11485,13 +11519,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11513,8 +11549,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H1" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>519</v>
       </c>
@@ -11532,7 +11571,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>519</v>
       </c>
@@ -11550,7 +11589,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>519</v>
       </c>
@@ -11570,7 +11609,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>519</v>
       </c>
@@ -11584,7 +11623,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>519</v>
       </c>
@@ -11598,7 +11637,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>519</v>
       </c>
@@ -11612,7 +11651,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>519</v>
       </c>
@@ -11626,7 +11665,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>519</v>
       </c>
@@ -11640,7 +11679,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>519</v>
       </c>
@@ -11654,7 +11693,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>519</v>
       </c>
@@ -11668,7 +11707,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>519</v>
       </c>
@@ -11682,7 +11721,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>519</v>
       </c>
@@ -11696,7 +11735,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>519</v>
       </c>
@@ -11710,7 +11749,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>519</v>
       </c>
@@ -11724,7 +11763,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>519</v>
       </c>
@@ -11748,9 +11787,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
@@ -11758,7 +11799,7 @@
     <col min="3" max="3" width="12.64453125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11780,8 +11821,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H1" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>527</v>
       </c>
@@ -11799,7 +11843,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>527</v>
       </c>
@@ -11817,7 +11861,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>527</v>
       </c>
@@ -11835,7 +11879,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>527</v>
       </c>
@@ -11855,7 +11899,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>527</v>
       </c>
@@ -11873,7 +11917,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>527</v>
       </c>
@@ -11893,7 +11937,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>527</v>
       </c>
@@ -11913,8 +11957,11 @@
       <c r="G8" s="2" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H8" s="1" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>527</v>
       </c>
@@ -11934,7 +11981,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>527</v>
       </c>
@@ -11948,7 +11995,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>527</v>
       </c>
@@ -11968,8 +12015,11 @@
       <c r="G11" s="2" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H11" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>527</v>
       </c>
@@ -11989,7 +12039,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>527</v>
       </c>
@@ -12003,7 +12053,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>527</v>
       </c>
@@ -12017,7 +12067,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>527</v>
       </c>
@@ -12031,7 +12081,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>527</v>
       </c>
@@ -12181,13 +12231,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12209,8 +12261,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H1" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>556</v>
       </c>
@@ -12225,8 +12280,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H2" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>556</v>
       </c>
@@ -12244,7 +12302,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>556</v>
       </c>
@@ -12258,7 +12316,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>556</v>
       </c>
@@ -12272,7 +12330,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>556</v>
       </c>
@@ -12286,7 +12344,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>556</v>
       </c>
@@ -12300,7 +12358,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>556</v>
       </c>
@@ -12314,7 +12372,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>556</v>
       </c>
@@ -12328,7 +12386,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>556</v>
       </c>
@@ -12342,7 +12400,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>556</v>
       </c>
@@ -12356,7 +12414,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>556</v>
       </c>
@@ -12370,7 +12428,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>556</v>
       </c>
@@ -12384,7 +12442,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>556</v>
       </c>
@@ -12398,7 +12456,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>556</v>
       </c>
@@ -12422,13 +12480,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12450,8 +12510,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H1" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>561</v>
       </c>
@@ -12466,8 +12529,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>561</v>
       </c>
@@ -12485,7 +12551,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>561</v>
       </c>
@@ -12503,7 +12569,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>561</v>
       </c>
@@ -12523,7 +12589,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>561</v>
       </c>
@@ -12541,7 +12607,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>561</v>
       </c>
@@ -12561,7 +12627,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>561</v>
       </c>
@@ -12575,7 +12641,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>561</v>
       </c>
@@ -12589,7 +12655,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>561</v>
       </c>
@@ -12603,7 +12669,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>561</v>
       </c>
@@ -12617,7 +12683,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>561</v>
       </c>
@@ -12631,7 +12697,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>561</v>
       </c>
@@ -12645,7 +12711,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>561</v>
       </c>
@@ -12659,7 +12725,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>561</v>
       </c>
@@ -12673,7 +12739,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>561</v>
       </c>
@@ -12739,13 +12805,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12767,8 +12835,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H1" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>575</v>
       </c>
@@ -12786,7 +12857,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>575</v>
       </c>
@@ -12804,7 +12875,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>575</v>
       </c>
@@ -12824,7 +12895,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>575</v>
       </c>
@@ -12838,7 +12909,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>575</v>
       </c>
@@ -12852,7 +12923,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>575</v>
       </c>
@@ -12866,7 +12937,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>575</v>
       </c>
@@ -12880,7 +12951,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>575</v>
       </c>
@@ -12894,7 +12965,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>575</v>
       </c>
@@ -12908,7 +12979,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>575</v>
       </c>
@@ -12922,7 +12993,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>575</v>
       </c>
@@ -12936,7 +13007,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>575</v>
       </c>
@@ -12950,7 +13021,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>575</v>
       </c>
@@ -12964,7 +13035,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>575</v>
       </c>
@@ -12978,7 +13049,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>575</v>
       </c>
@@ -13002,16 +13073,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="3" max="3" width="12.64453125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13033,8 +13106,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H1" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>583</v>
       </c>
@@ -13052,7 +13128,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>583</v>
       </c>
@@ -13070,7 +13146,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>583</v>
       </c>
@@ -13088,7 +13164,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>583</v>
       </c>
@@ -13106,7 +13182,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>583</v>
       </c>
@@ -13124,7 +13200,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>583</v>
       </c>
@@ -13142,7 +13218,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>583</v>
       </c>
@@ -13160,7 +13236,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>583</v>
       </c>
@@ -13180,7 +13256,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>583</v>
       </c>
@@ -13198,7 +13274,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>583</v>
       </c>
@@ -13216,7 +13292,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
         <v>583</v>
       </c>
@@ -13236,7 +13312,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>583</v>
       </c>
@@ -13254,7 +13330,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
         <v>583</v>
       </c>
@@ -13272,7 +13348,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>583</v>
       </c>
@@ -13290,7 +13366,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>583</v>
       </c>
@@ -13308,7 +13384,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>583</v>
       </c>
@@ -13326,7 +13402,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>583</v>
       </c>
@@ -13344,7 +13420,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>583</v>
       </c>
@@ -13364,7 +13440,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>583</v>
       </c>
@@ -13381,8 +13457,11 @@
         <v>28</v>
       </c>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="H20" s="1" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
         <v>583</v>
       </c>
@@ -13402,7 +13481,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A22" s="2" t="s">
         <v>583</v>
       </c>
@@ -13418,7 +13497,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A23" s="2" t="s">
         <v>583</v>
       </c>
@@ -13436,7 +13515,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A24" s="2" t="s">
         <v>583</v>
       </c>
@@ -13456,7 +13535,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A25" s="2" t="s">
         <v>583</v>
       </c>
@@ -13476,7 +13555,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
         <v>583</v>
       </c>
@@ -13496,7 +13575,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A27" s="2" t="s">
         <v>583</v>
       </c>
@@ -13514,7 +13593,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A28" s="2" t="s">
         <v>583</v>
       </c>
@@ -13534,7 +13613,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A29" s="2" t="s">
         <v>583</v>
       </c>
@@ -13552,7 +13631,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A30" s="2" t="s">
         <v>583</v>
       </c>
@@ -13570,7 +13649,7 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A31" s="2" t="s">
         <v>583</v>
       </c>
@@ -13588,7 +13667,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" ht="14.35" x14ac:dyDescent="0.5">
       <c r="A32" s="2" t="s">
         <v>583</v>
       </c>

</xml_diff>